<commit_message>
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C768915
</commit_message>
<xml_diff>
--- a/PPIUK-KHPADD/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-KHPADD/src/test/resources/CobaltUsers.xlsx
@@ -1054,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G84"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="G84" sqref="A81:G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2577,18 +2577,6 @@
       <c r="G80" s="10" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E81" s="9"/>
-    </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E82" s="9"/>
-    </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E83" s="9"/>
-    </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E84" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Yuri - new test for bug 848107
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C773543
</commit_message>
<xml_diff>
--- a/PPIUK-KHPADD/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-KHPADD/src/test/resources/CobaltUsers.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="277">
   <si>
     <t>UserName</t>
   </si>
@@ -838,6 +838,15 @@
   </si>
   <si>
     <t xml:space="preserve">AssetPageUser5@mailinator.com </t>
+  </si>
+  <si>
+    <t>LimitedSubscriptionsUser</t>
+  </si>
+  <si>
+    <t>User with access for Employment only</t>
+  </si>
+  <si>
+    <t>LimitedSubscriptionsUser@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -1014,7 +1023,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1049,7 +1058,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1258,10 +1267,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G113"/>
+  <dimension ref="A1:G114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81:G113"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E113" sqref="E113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3341,6 +3350,20 @@
       </c>
       <c r="G113" s="10" t="s">
         <v>273</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>274</v>
+      </c>
+      <c r="B114" t="s">
+        <v>52</v>
+      </c>
+      <c r="E114" t="s">
+        <v>275</v>
+      </c>
+      <c r="G114" t="s">
+        <v>276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Usman - New runner for KHPadd
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C773665
</commit_message>
<xml_diff>
--- a/PPIUK-KHPADD/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-KHPADD/src/test/resources/CobaltUsers.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="278">
   <si>
     <t>UserName</t>
   </si>
@@ -447,9 +447,6 @@
     <t>anztestuser4@mailinator.com</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>Linking_AutoUser</t>
   </si>
   <si>
@@ -847,6 +844,12 @@
   </si>
   <si>
     <t>LimitedSubscriptionsUser@mailinator.com</t>
+  </si>
+  <si>
+    <t>KHPaddUser7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KHPaddUser7@mailinator.com </t>
   </si>
 </sst>
 </file>
@@ -1023,7 +1026,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1058,7 +1061,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1267,10 +1270,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G114"/>
+  <dimension ref="A1:G115"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E113" sqref="E113"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="G115" sqref="G115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2298,7 +2301,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>52</v>
@@ -2306,1064 +2309,1081 @@
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G52" s="5" t="s">
         <v>145</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B53" t="s">
         <v>52</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F53" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B54" t="s">
         <v>52</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F54" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B55" t="s">
         <v>52</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F55" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G55" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B56" t="s">
         <v>52</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F56" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B57" t="s">
         <v>52</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F57" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B58" t="s">
         <v>52</v>
       </c>
       <c r="E58" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F58" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B59" t="s">
         <v>52</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F59" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B60" t="s">
         <v>52</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F60" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B61" t="s">
         <v>52</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F61" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B62" t="s">
         <v>52</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F62" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B63" t="s">
         <v>52</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F63" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B64" t="s">
         <v>52</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F64" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G64" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B65" t="s">
         <v>52</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F65" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B66" t="s">
         <v>52</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F66" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B67" t="s">
         <v>52</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F67" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G67" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B68" t="s">
         <v>52</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F68" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G68" s="10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B69" t="s">
         <v>52</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F69" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G69" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B70" t="s">
         <v>52</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F70" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G70" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B71" t="s">
         <v>52</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F71" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G71" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B72" t="s">
         <v>52</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F72" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G72" s="10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B73" t="s">
         <v>52</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F73" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G73" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B74" t="s">
         <v>52</v>
       </c>
       <c r="E74" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F74" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G74" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B75" t="s">
         <v>52</v>
       </c>
       <c r="E75" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F75" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G75" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B76" t="s">
         <v>52</v>
       </c>
       <c r="E76" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F76" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G76" s="10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B77" t="s">
         <v>52</v>
       </c>
       <c r="E77" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F77" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G77" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B78" t="s">
         <v>52</v>
       </c>
       <c r="E78" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F78" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G78" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B79" t="s">
         <v>52</v>
       </c>
       <c r="E79" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F79" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G79" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B80" t="s">
         <v>52</v>
       </c>
       <c r="E80" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F80" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G80" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="B81" t="s">
+        <v>52</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F81" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G81" s="10" t="s">
         <v>208</v>
-      </c>
-      <c r="B81" t="s">
-        <v>52</v>
-      </c>
-      <c r="E81" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F81" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G81" s="10" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="B82" t="s">
+        <v>52</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F82" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G82" s="10" t="s">
         <v>210</v>
-      </c>
-      <c r="B82" t="s">
-        <v>52</v>
-      </c>
-      <c r="E82" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F82" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G82" s="10" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="B83" t="s">
+        <v>52</v>
+      </c>
+      <c r="E83" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F83" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G83" s="10" t="s">
         <v>212</v>
-      </c>
-      <c r="B83" t="s">
-        <v>52</v>
-      </c>
-      <c r="E83" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F83" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G83" s="10" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="B84" t="s">
+        <v>52</v>
+      </c>
+      <c r="E84" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F84" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G84" s="10" t="s">
         <v>214</v>
-      </c>
-      <c r="B84" t="s">
-        <v>52</v>
-      </c>
-      <c r="E84" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F84" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G84" s="10" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="B85" t="s">
+        <v>52</v>
+      </c>
+      <c r="E85" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F85" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G85" s="10" t="s">
         <v>216</v>
-      </c>
-      <c r="B85" t="s">
-        <v>52</v>
-      </c>
-      <c r="E85" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F85" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G85" s="10" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="B86" t="s">
+        <v>52</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F86" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G86" s="10" t="s">
         <v>218</v>
-      </c>
-      <c r="B86" t="s">
-        <v>52</v>
-      </c>
-      <c r="E86" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F86" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G86" s="10" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="B87" t="s">
+        <v>52</v>
+      </c>
+      <c r="E87" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F87" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G87" s="10" t="s">
         <v>220</v>
-      </c>
-      <c r="B87" t="s">
-        <v>52</v>
-      </c>
-      <c r="E87" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F87" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G87" s="10" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="B88" t="s">
+        <v>52</v>
+      </c>
+      <c r="E88" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F88" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G88" s="10" t="s">
         <v>222</v>
-      </c>
-      <c r="B88" t="s">
-        <v>52</v>
-      </c>
-      <c r="E88" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F88" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G88" s="10" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="11" t="s">
+        <v>223</v>
+      </c>
+      <c r="B89" t="s">
+        <v>52</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F89" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G89" s="10" t="s">
         <v>224</v>
-      </c>
-      <c r="B89" t="s">
-        <v>52</v>
-      </c>
-      <c r="E89" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F89" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G89" s="10" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="B90" t="s">
+        <v>52</v>
+      </c>
+      <c r="E90" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F90" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G90" s="10" t="s">
         <v>226</v>
-      </c>
-      <c r="B90" t="s">
-        <v>52</v>
-      </c>
-      <c r="E90" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F90" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G90" s="10" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="B91" t="s">
+        <v>52</v>
+      </c>
+      <c r="E91" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F91" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G91" s="10" t="s">
         <v>228</v>
-      </c>
-      <c r="B91" t="s">
-        <v>52</v>
-      </c>
-      <c r="E91" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F91" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G91" s="10" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="B92" t="s">
+        <v>52</v>
+      </c>
+      <c r="E92" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F92" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G92" s="10" t="s">
         <v>230</v>
-      </c>
-      <c r="B92" t="s">
-        <v>52</v>
-      </c>
-      <c r="E92" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F92" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G92" s="10" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="B93" t="s">
+        <v>52</v>
+      </c>
+      <c r="E93" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F93" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G93" s="10" t="s">
         <v>232</v>
-      </c>
-      <c r="B93" t="s">
-        <v>52</v>
-      </c>
-      <c r="E93" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F93" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G93" s="10" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="B94" t="s">
+        <v>52</v>
+      </c>
+      <c r="E94" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F94" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G94" s="10" t="s">
         <v>234</v>
-      </c>
-      <c r="B94" t="s">
-        <v>52</v>
-      </c>
-      <c r="E94" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F94" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G94" s="10" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="B95" t="s">
+        <v>52</v>
+      </c>
+      <c r="E95" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F95" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G95" s="10" t="s">
         <v>236</v>
-      </c>
-      <c r="B95" t="s">
-        <v>52</v>
-      </c>
-      <c r="E95" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F95" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G95" s="10" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="B96" t="s">
+        <v>52</v>
+      </c>
+      <c r="E96" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F96" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G96" s="10" t="s">
         <v>238</v>
-      </c>
-      <c r="B96" t="s">
-        <v>52</v>
-      </c>
-      <c r="E96" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F96" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G96" s="10" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="B97" t="s">
+        <v>52</v>
+      </c>
+      <c r="E97" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F97" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G97" s="10" t="s">
         <v>240</v>
-      </c>
-      <c r="B97" t="s">
-        <v>52</v>
-      </c>
-      <c r="E97" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F97" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G97" s="10" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="B98" t="s">
+        <v>52</v>
+      </c>
+      <c r="E98" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F98" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G98" s="10" t="s">
         <v>242</v>
-      </c>
-      <c r="B98" t="s">
-        <v>52</v>
-      </c>
-      <c r="E98" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F98" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G98" s="10" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="B99" t="s">
+        <v>52</v>
+      </c>
+      <c r="E99" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F99" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G99" s="10" t="s">
         <v>244</v>
-      </c>
-      <c r="B99" t="s">
-        <v>52</v>
-      </c>
-      <c r="E99" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F99" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G99" s="10" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="B100" t="s">
+        <v>52</v>
+      </c>
+      <c r="E100" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F100" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G100" s="10" t="s">
         <v>246</v>
-      </c>
-      <c r="B100" t="s">
-        <v>52</v>
-      </c>
-      <c r="E100" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F100" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G100" s="10" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="B101" t="s">
+        <v>52</v>
+      </c>
+      <c r="E101" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F101" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G101" s="10" t="s">
         <v>248</v>
-      </c>
-      <c r="B101" t="s">
-        <v>52</v>
-      </c>
-      <c r="E101" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F101" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G101" s="10" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="B102" t="s">
+        <v>52</v>
+      </c>
+      <c r="E102" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F102" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G102" s="10" t="s">
         <v>250</v>
-      </c>
-      <c r="B102" t="s">
-        <v>52</v>
-      </c>
-      <c r="E102" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F102" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G102" s="10" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="B103" t="s">
+        <v>52</v>
+      </c>
+      <c r="E103" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F103" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G103" s="10" t="s">
         <v>252</v>
-      </c>
-      <c r="B103" t="s">
-        <v>52</v>
-      </c>
-      <c r="E103" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F103" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G103" s="10" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="B104" t="s">
+        <v>52</v>
+      </c>
+      <c r="E104" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F104" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G104" s="10" t="s">
         <v>254</v>
-      </c>
-      <c r="B104" t="s">
-        <v>52</v>
-      </c>
-      <c r="E104" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F104" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G104" s="10" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="B105" t="s">
+        <v>52</v>
+      </c>
+      <c r="E105" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F105" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G105" s="10" t="s">
         <v>256</v>
-      </c>
-      <c r="B105" t="s">
-        <v>52</v>
-      </c>
-      <c r="E105" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F105" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G105" s="10" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="B106" t="s">
+        <v>52</v>
+      </c>
+      <c r="E106" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F106" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G106" s="10" t="s">
         <v>258</v>
-      </c>
-      <c r="B106" t="s">
-        <v>52</v>
-      </c>
-      <c r="E106" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F106" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G106" s="10" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
+        <v>259</v>
+      </c>
+      <c r="B107" t="s">
+        <v>52</v>
+      </c>
+      <c r="E107" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F107" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G107" s="10" t="s">
         <v>260</v>
-      </c>
-      <c r="B107" t="s">
-        <v>52</v>
-      </c>
-      <c r="E107" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F107" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G107" s="10" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="B108" t="s">
+        <v>52</v>
+      </c>
+      <c r="E108" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F108" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G108" s="10" t="s">
         <v>262</v>
-      </c>
-      <c r="B108" t="s">
-        <v>52</v>
-      </c>
-      <c r="E108" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F108" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G108" s="10" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="B109" t="s">
+        <v>52</v>
+      </c>
+      <c r="E109" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F109" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G109" s="10" t="s">
         <v>264</v>
-      </c>
-      <c r="B109" t="s">
-        <v>52</v>
-      </c>
-      <c r="E109" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F109" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G109" s="10" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="B110" t="s">
+        <v>52</v>
+      </c>
+      <c r="E110" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F110" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G110" s="10" t="s">
         <v>266</v>
-      </c>
-      <c r="B110" t="s">
-        <v>52</v>
-      </c>
-      <c r="E110" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F110" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G110" s="10" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="B111" t="s">
+        <v>52</v>
+      </c>
+      <c r="E111" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F111" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G111" s="10" t="s">
         <v>268</v>
-      </c>
-      <c r="B111" t="s">
-        <v>52</v>
-      </c>
-      <c r="E111" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F111" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G111" s="10" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="B112" t="s">
+        <v>52</v>
+      </c>
+      <c r="E112" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F112" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G112" s="10" t="s">
         <v>270</v>
-      </c>
-      <c r="B112" t="s">
-        <v>52</v>
-      </c>
-      <c r="E112" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F112" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G112" s="10" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="B113" t="s">
+        <v>52</v>
+      </c>
+      <c r="E113" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="F113" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G113" s="10" t="s">
         <v>272</v>
-      </c>
-      <c r="B113" t="s">
-        <v>52</v>
-      </c>
-      <c r="E113" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="F113" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G113" s="10" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>273</v>
+      </c>
+      <c r="B114" t="s">
+        <v>52</v>
+      </c>
+      <c r="E114" t="s">
         <v>274</v>
       </c>
-      <c r="B114" t="s">
-        <v>52</v>
-      </c>
-      <c r="E114" t="s">
+      <c r="G114" t="s">
         <v>275</v>
       </c>
-      <c r="G114" t="s">
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" s="11" t="s">
         <v>276</v>
+      </c>
+      <c r="B115" t="s">
+        <v>52</v>
+      </c>
+      <c r="E115" t="s">
+        <v>202</v>
+      </c>
+      <c r="F115" t="s">
+        <v>25</v>
+      </c>
+      <c r="G115" s="10" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -3444,9 +3464,10 @@
     <hyperlink ref="G110" r:id="rId74"/>
     <hyperlink ref="G113" r:id="rId75"/>
     <hyperlink ref="G111" r:id="rId76" display="AssetPageUser1@mailinator.com "/>
+    <hyperlink ref="G115" r:id="rId77"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId77"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId78"/>
 </worksheet>
 </file>
 
@@ -3460,8 +3481,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -3469,23 +3490,23 @@
         <v>68</v>
       </c>
       <c r="B1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B2" t="s">
         <v>205</v>
-      </c>
-      <c r="B2" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -3495,18 +3516,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Kostya - KHPADD - FacetCount refactor
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C776494
</commit_message>
<xml_diff>
--- a/PPIUK-KHPADD/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-KHPADD/src/test/resources/CobaltUsers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="279">
   <si>
     <t>UserName</t>
   </si>
@@ -850,13 +850,17 @@
   </si>
   <si>
     <t xml:space="preserve">KHPaddUser7@mailinator.com </t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1278,12 +1282,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="40.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3481,8 +3485,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Yury Karol - added user Yury_Karol for Release Team purposes
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C794652
</commit_message>
<xml_diff>
--- a/PPIUK-KHPADD/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-KHPADD/src/test/resources/CobaltUsers.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="284">
   <si>
     <t>UserName</t>
   </si>
@@ -859,6 +859,15 @@
   </si>
   <si>
     <t>Password!</t>
+  </si>
+  <si>
+    <t>Yury_Karol</t>
+  </si>
+  <si>
+    <t>Password!1</t>
+  </si>
+  <si>
+    <t>END2END User</t>
   </si>
 </sst>
 </file>
@@ -1279,23 +1288,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G116"/>
+  <dimension ref="A1:G117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="21.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="27.44140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="39.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="40.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1318,7 +1327,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -1339,7 +1348,7 @@
       </c>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1358,7 +1367,7 @@
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -1377,7 +1386,7 @@
       </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -1398,7 +1407,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1419,7 +1428,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1440,7 +1449,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1461,7 +1470,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>279</v>
       </c>
@@ -1480,7 +1489,7 @@
       </c>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
@@ -1501,7 +1510,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -1522,7 +1531,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>38</v>
       </c>
@@ -1543,7 +1552,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>39</v>
       </c>
@@ -1564,7 +1573,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>40</v>
       </c>
@@ -1583,7 +1592,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>41</v>
       </c>
@@ -1604,7 +1613,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
@@ -1625,7 +1634,7 @@
       </c>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
@@ -1644,7 +1653,7 @@
       </c>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>31</v>
       </c>
@@ -1665,7 +1674,7 @@
       </c>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>36</v>
       </c>
@@ -1684,7 +1693,7 @@
       </c>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>47</v>
       </c>
@@ -1703,7 +1712,7 @@
       </c>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>50</v>
       </c>
@@ -1722,7 +1731,7 @@
       </c>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>51</v>
       </c>
@@ -1743,7 +1752,7 @@
       </c>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>53</v>
       </c>
@@ -1764,7 +1773,7 @@
       </c>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>120</v>
       </c>
@@ -1783,7 +1792,7 @@
       </c>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>56</v>
       </c>
@@ -1802,7 +1811,7 @@
       </c>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>57</v>
       </c>
@@ -1819,7 +1828,7 @@
       </c>
       <c r="G26" s="5"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>59</v>
       </c>
@@ -1836,7 +1845,7 @@
       </c>
       <c r="G27" s="5"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>61</v>
       </c>
@@ -1855,7 +1864,7 @@
       </c>
       <c r="G28" s="5"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>63</v>
       </c>
@@ -1872,7 +1881,7 @@
       </c>
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>65</v>
       </c>
@@ -1889,7 +1898,7 @@
       </c>
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>277</v>
       </c>
@@ -1908,47 +1917,47 @@
       </c>
       <c r="G31" s="5"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>74</v>
+        <v>281</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>52</v>
+        <v>282</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5" t="s">
         <v>21</v>
       </c>
       <c r="E32" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="F32" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G32" s="5"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+      <c r="F33" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>84</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>81</v>
@@ -1956,134 +1965,130 @@
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F34" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G34" s="5" t="s">
+      <c r="F35" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5" t="s">
+      <c r="B36" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G35" s="6" t="s">
+      <c r="E36" s="5"/>
+      <c r="F36" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G36" s="6" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
+      <c r="E37" s="5" t="s">
+        <v>91</v>
+      </c>
       <c r="F37" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>52</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
-      <c r="E38" s="5" t="s">
-        <v>122</v>
-      </c>
+      <c r="E38" s="5"/>
       <c r="F38" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
       <c r="E39" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="F39" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G39" s="5" t="s">
+      <c r="F40" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G40" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>103</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>52</v>
@@ -2095,121 +2100,125 @@
         <v>33</v>
       </c>
       <c r="E41" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E42" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="F41" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G41" s="6" t="s">
+      <c r="F42" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G42" s="6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B43" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5" t="s">
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="F42" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G42" s="6" t="s">
+      <c r="F43" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G43" s="6" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B43" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C43" s="5" t="s">
+      <c r="B44" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D44" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E44" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="F43" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G43" s="5"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+      <c r="F44" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G44" s="5"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B44" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C44" s="5" t="s">
+      <c r="B45" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D45" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="E45" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="F44" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G44" s="5"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
+      <c r="F45" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G45" s="5"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B45" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C45" s="5" t="s">
+      <c r="B46" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D46" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="E46" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F45" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G45" s="5" t="s">
+      <c r="F46" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G46" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
         <v>116</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G46" s="8" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
-        <v>117</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>52</v>
@@ -2223,94 +2232,94 @@
         <v>25</v>
       </c>
       <c r="G47" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G48" s="8" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B49" s="5" t="s">
         <v>124</v>
-      </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>129</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>25</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="E50" s="5" t="s">
+      <c r="E51" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="F50" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G50" s="6" t="s">
+      <c r="F51" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G51" s="6" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
         <v>138</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G51" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
-        <v>140</v>
       </c>
       <c r="B52" s="5" t="s">
         <v>52</v>
@@ -2324,12 +2333,12 @@
         <v>25</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B53" s="5" t="s">
         <v>52</v>
@@ -2337,1080 +2346,1099 @@
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="F53" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G53" s="5" t="s">
+      <c r="F54" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G54" s="5" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>145</v>
       </c>
-      <c r="B54" t="s">
-        <v>52</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F54" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G54" s="10" t="s">
+      <c r="B55" t="s">
+        <v>52</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G55" s="10" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>146</v>
       </c>
-      <c r="B55" t="s">
-        <v>52</v>
-      </c>
-      <c r="E55" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F55" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G55" s="10" t="s">
+      <c r="B56" t="s">
+        <v>52</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G56" s="10" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>147</v>
       </c>
-      <c r="B56" t="s">
-        <v>52</v>
-      </c>
-      <c r="E56" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F56" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G56" s="10" t="s">
+      <c r="B57" t="s">
+        <v>52</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G57" s="10" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>148</v>
       </c>
-      <c r="B57" t="s">
-        <v>52</v>
-      </c>
-      <c r="E57" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F57" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G57" s="10" t="s">
+      <c r="B58" t="s">
+        <v>52</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F58" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G58" s="10" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>149</v>
       </c>
-      <c r="B58" t="s">
-        <v>52</v>
-      </c>
-      <c r="E58" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F58" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G58" s="10" t="s">
+      <c r="B59" t="s">
+        <v>52</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G59" s="10" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>150</v>
       </c>
-      <c r="B59" t="s">
-        <v>52</v>
-      </c>
-      <c r="E59" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F59" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G59" s="10" t="s">
+      <c r="B60" t="s">
+        <v>52</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G60" s="10" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>151</v>
       </c>
-      <c r="B60" t="s">
-        <v>52</v>
-      </c>
-      <c r="E60" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F60" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G60" s="10" t="s">
+      <c r="B61" t="s">
+        <v>52</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G61" s="10" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>152</v>
       </c>
-      <c r="B61" t="s">
-        <v>52</v>
-      </c>
-      <c r="E61" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F61" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G61" s="10" t="s">
+      <c r="B62" t="s">
+        <v>52</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F62" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G62" s="10" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>153</v>
       </c>
-      <c r="B62" t="s">
-        <v>52</v>
-      </c>
-      <c r="E62" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F62" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G62" s="10" t="s">
+      <c r="B63" t="s">
+        <v>52</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F63" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G63" s="10" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>154</v>
       </c>
-      <c r="B63" t="s">
-        <v>52</v>
-      </c>
-      <c r="E63" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F63" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G63" s="10" t="s">
+      <c r="B64" t="s">
+        <v>52</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F64" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G64" s="10" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>155</v>
       </c>
-      <c r="B64" t="s">
-        <v>52</v>
-      </c>
-      <c r="E64" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F64" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G64" s="10" t="s">
+      <c r="B65" t="s">
+        <v>52</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F65" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G65" s="10" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>156</v>
       </c>
-      <c r="B65" t="s">
-        <v>52</v>
-      </c>
-      <c r="E65" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F65" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G65" s="10" t="s">
+      <c r="B66" t="s">
+        <v>52</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F66" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G66" s="10" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>157</v>
       </c>
-      <c r="B66" t="s">
-        <v>52</v>
-      </c>
-      <c r="E66" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F66" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G66" s="10" t="s">
+      <c r="B67" t="s">
+        <v>52</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F67" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G67" s="10" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>158</v>
       </c>
-      <c r="B67" t="s">
-        <v>52</v>
-      </c>
-      <c r="E67" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F67" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G67" s="10" t="s">
+      <c r="B68" t="s">
+        <v>52</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F68" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G68" s="10" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>159</v>
       </c>
-      <c r="B68" t="s">
-        <v>52</v>
-      </c>
-      <c r="E68" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F68" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G68" s="10" t="s">
+      <c r="B69" t="s">
+        <v>52</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G69" s="10" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
         <v>160</v>
       </c>
-      <c r="B69" t="s">
-        <v>52</v>
-      </c>
-      <c r="E69" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F69" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G69" s="10" t="s">
+      <c r="B70" t="s">
+        <v>52</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F70" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G70" s="10" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
         <v>161</v>
       </c>
-      <c r="B70" t="s">
-        <v>52</v>
-      </c>
-      <c r="E70" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F70" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G70" s="10" t="s">
+      <c r="B71" t="s">
+        <v>52</v>
+      </c>
+      <c r="E71" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F71" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G71" s="10" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
         <v>162</v>
       </c>
-      <c r="B71" t="s">
-        <v>52</v>
-      </c>
-      <c r="E71" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F71" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G71" s="10" t="s">
+      <c r="B72" t="s">
+        <v>52</v>
+      </c>
+      <c r="E72" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F72" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G72" s="10" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
         <v>163</v>
       </c>
-      <c r="B72" t="s">
-        <v>52</v>
-      </c>
-      <c r="E72" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F72" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G72" s="10" t="s">
+      <c r="B73" t="s">
+        <v>52</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G73" s="10" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>164</v>
       </c>
-      <c r="B73" t="s">
-        <v>52</v>
-      </c>
-      <c r="E73" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F73" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G73" s="10" t="s">
+      <c r="B74" t="s">
+        <v>52</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F74" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G74" s="10" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>165</v>
       </c>
-      <c r="B74" t="s">
-        <v>52</v>
-      </c>
-      <c r="E74" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F74" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G74" s="10" t="s">
+      <c r="B75" t="s">
+        <v>52</v>
+      </c>
+      <c r="E75" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F75" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G75" s="10" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
         <v>166</v>
       </c>
-      <c r="B75" t="s">
-        <v>52</v>
-      </c>
-      <c r="E75" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F75" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G75" s="10" t="s">
+      <c r="B76" t="s">
+        <v>52</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F76" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G76" s="10" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
         <v>167</v>
       </c>
-      <c r="B76" t="s">
-        <v>52</v>
-      </c>
-      <c r="E76" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F76" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G76" s="10" t="s">
+      <c r="B77" t="s">
+        <v>52</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F77" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G77" s="10" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>168</v>
       </c>
-      <c r="B77" t="s">
-        <v>52</v>
-      </c>
-      <c r="E77" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F77" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G77" s="10" t="s">
+      <c r="B78" t="s">
+        <v>52</v>
+      </c>
+      <c r="E78" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F78" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G78" s="10" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>169</v>
       </c>
-      <c r="B78" t="s">
-        <v>52</v>
-      </c>
-      <c r="E78" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F78" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G78" s="10" t="s">
+      <c r="B79" t="s">
+        <v>52</v>
+      </c>
+      <c r="E79" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F79" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G79" s="10" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>170</v>
       </c>
-      <c r="B79" t="s">
-        <v>52</v>
-      </c>
-      <c r="E79" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F79" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G79" s="10" t="s">
+      <c r="B80" t="s">
+        <v>52</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F80" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G80" s="10" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
         <v>171</v>
       </c>
-      <c r="B80" t="s">
-        <v>52</v>
-      </c>
-      <c r="E80" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F80" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G80" s="10" t="s">
+      <c r="B81" t="s">
+        <v>52</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F81" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G81" s="10" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
         <v>172</v>
       </c>
-      <c r="B81" t="s">
-        <v>52</v>
-      </c>
-      <c r="E81" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F81" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G81" s="10" t="s">
+      <c r="B82" t="s">
+        <v>52</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F82" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G82" s="10" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="11" t="s">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A83" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="B82" t="s">
-        <v>52</v>
-      </c>
-      <c r="E82" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F82" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G82" s="10" t="s">
+      <c r="B83" t="s">
+        <v>52</v>
+      </c>
+      <c r="E83" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F83" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G83" s="10" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="11" t="s">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A84" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="B83" t="s">
-        <v>52</v>
-      </c>
-      <c r="E83" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F83" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G83" s="10" t="s">
+      <c r="B84" t="s">
+        <v>52</v>
+      </c>
+      <c r="E84" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F84" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G84" s="10" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="11" t="s">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A85" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="B84" t="s">
-        <v>52</v>
-      </c>
-      <c r="E84" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F84" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G84" s="10" t="s">
+      <c r="B85" t="s">
+        <v>52</v>
+      </c>
+      <c r="E85" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F85" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G85" s="10" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="11" t="s">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A86" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="B85" t="s">
-        <v>52</v>
-      </c>
-      <c r="E85" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F85" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G85" s="10" t="s">
+      <c r="B86" t="s">
+        <v>52</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F86" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G86" s="10" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="11" t="s">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A87" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="B86" t="s">
-        <v>52</v>
-      </c>
-      <c r="E86" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F86" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G86" s="10" t="s">
+      <c r="B87" t="s">
+        <v>52</v>
+      </c>
+      <c r="E87" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F87" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G87" s="10" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="11" t="s">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A88" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="B87" t="s">
-        <v>52</v>
-      </c>
-      <c r="E87" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F87" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G87" s="10" t="s">
+      <c r="B88" t="s">
+        <v>52</v>
+      </c>
+      <c r="E88" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F88" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G88" s="10" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="11" t="s">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A89" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="B88" t="s">
-        <v>52</v>
-      </c>
-      <c r="E88" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F88" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G88" s="10" t="s">
+      <c r="B89" t="s">
+        <v>52</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F89" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G89" s="10" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="11" t="s">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A90" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="B89" t="s">
-        <v>52</v>
-      </c>
-      <c r="E89" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F89" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G89" s="10" t="s">
+      <c r="B90" t="s">
+        <v>52</v>
+      </c>
+      <c r="E90" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F90" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G90" s="10" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="11" t="s">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A91" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="B90" t="s">
-        <v>52</v>
-      </c>
-      <c r="E90" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F90" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G90" s="10" t="s">
+      <c r="B91" t="s">
+        <v>52</v>
+      </c>
+      <c r="E91" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F91" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G91" s="10" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="11" t="s">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A92" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="B91" t="s">
-        <v>52</v>
-      </c>
-      <c r="E91" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F91" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G91" s="10" t="s">
+      <c r="B92" t="s">
+        <v>52</v>
+      </c>
+      <c r="E92" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F92" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G92" s="10" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="11" t="s">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A93" s="11" t="s">
         <v>226</v>
       </c>
-      <c r="B92" t="s">
-        <v>52</v>
-      </c>
-      <c r="E92" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F92" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G92" s="10" t="s">
+      <c r="B93" t="s">
+        <v>52</v>
+      </c>
+      <c r="E93" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F93" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G93" s="10" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="11" t="s">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A94" s="11" t="s">
         <v>228</v>
       </c>
-      <c r="B93" t="s">
-        <v>52</v>
-      </c>
-      <c r="E93" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F93" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G93" s="10" t="s">
+      <c r="B94" t="s">
+        <v>52</v>
+      </c>
+      <c r="E94" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F94" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G94" s="10" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="11" t="s">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A95" s="11" t="s">
         <v>230</v>
       </c>
-      <c r="B94" t="s">
-        <v>52</v>
-      </c>
-      <c r="E94" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F94" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G94" s="10" t="s">
+      <c r="B95" t="s">
+        <v>52</v>
+      </c>
+      <c r="E95" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F95" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G95" s="10" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="11" t="s">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A96" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="B95" t="s">
-        <v>52</v>
-      </c>
-      <c r="E95" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F95" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G95" s="10" t="s">
+      <c r="B96" t="s">
+        <v>52</v>
+      </c>
+      <c r="E96" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F96" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G96" s="10" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="11" t="s">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A97" s="11" t="s">
         <v>234</v>
       </c>
-      <c r="B96" t="s">
-        <v>52</v>
-      </c>
-      <c r="E96" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F96" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G96" s="10" t="s">
+      <c r="B97" t="s">
+        <v>52</v>
+      </c>
+      <c r="E97" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F97" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G97" s="10" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="11" t="s">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A98" s="11" t="s">
         <v>236</v>
       </c>
-      <c r="B97" t="s">
-        <v>52</v>
-      </c>
-      <c r="E97" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F97" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G97" s="10" t="s">
+      <c r="B98" t="s">
+        <v>52</v>
+      </c>
+      <c r="E98" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F98" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G98" s="10" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="11" t="s">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A99" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="B98" t="s">
-        <v>52</v>
-      </c>
-      <c r="E98" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F98" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G98" s="10" t="s">
+      <c r="B99" t="s">
+        <v>52</v>
+      </c>
+      <c r="E99" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F99" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G99" s="10" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="11" t="s">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A100" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="B99" t="s">
-        <v>52</v>
-      </c>
-      <c r="E99" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F99" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G99" s="10" t="s">
+      <c r="B100" t="s">
+        <v>52</v>
+      </c>
+      <c r="E100" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F100" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G100" s="10" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="11" t="s">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A101" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="B100" t="s">
-        <v>52</v>
-      </c>
-      <c r="E100" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F100" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G100" s="10" t="s">
+      <c r="B101" t="s">
+        <v>52</v>
+      </c>
+      <c r="E101" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F101" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G101" s="10" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="11" t="s">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A102" s="11" t="s">
         <v>244</v>
       </c>
-      <c r="B101" t="s">
-        <v>52</v>
-      </c>
-      <c r="E101" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F101" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G101" s="10" t="s">
+      <c r="B102" t="s">
+        <v>52</v>
+      </c>
+      <c r="E102" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F102" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G102" s="10" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="11" t="s">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A103" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="B102" t="s">
-        <v>52</v>
-      </c>
-      <c r="E102" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F102" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G102" s="10" t="s">
+      <c r="B103" t="s">
+        <v>52</v>
+      </c>
+      <c r="E103" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F103" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G103" s="10" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="11" t="s">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A104" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="B103" t="s">
-        <v>52</v>
-      </c>
-      <c r="E103" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F103" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G103" s="10" t="s">
+      <c r="B104" t="s">
+        <v>52</v>
+      </c>
+      <c r="E104" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F104" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G104" s="10" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="11" t="s">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A105" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="B104" t="s">
-        <v>52</v>
-      </c>
-      <c r="E104" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F104" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G104" s="10" t="s">
+      <c r="B105" t="s">
+        <v>52</v>
+      </c>
+      <c r="E105" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F105" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G105" s="10" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="11" t="s">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A106" s="11" t="s">
         <v>252</v>
       </c>
-      <c r="B105" t="s">
-        <v>52</v>
-      </c>
-      <c r="E105" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F105" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G105" s="10" t="s">
+      <c r="B106" t="s">
+        <v>52</v>
+      </c>
+      <c r="E106" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F106" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G106" s="10" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="11" t="s">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A107" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="B106" t="s">
-        <v>52</v>
-      </c>
-      <c r="E106" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F106" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G106" s="10" t="s">
+      <c r="B107" t="s">
+        <v>52</v>
+      </c>
+      <c r="E107" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F107" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G107" s="10" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="11" t="s">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A108" s="11" t="s">
         <v>256</v>
       </c>
-      <c r="B107" t="s">
-        <v>52</v>
-      </c>
-      <c r="E107" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F107" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G107" s="10" t="s">
+      <c r="B108" t="s">
+        <v>52</v>
+      </c>
+      <c r="E108" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F108" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G108" s="10" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="11" t="s">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A109" s="11" t="s">
         <v>258</v>
       </c>
-      <c r="B108" t="s">
-        <v>52</v>
-      </c>
-      <c r="E108" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F108" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G108" s="10" t="s">
+      <c r="B109" t="s">
+        <v>52</v>
+      </c>
+      <c r="E109" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F109" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G109" s="10" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="11" t="s">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A110" s="11" t="s">
         <v>260</v>
       </c>
-      <c r="B109" t="s">
-        <v>52</v>
-      </c>
-      <c r="E109" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F109" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G109" s="10" t="s">
+      <c r="B110" t="s">
+        <v>52</v>
+      </c>
+      <c r="E110" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F110" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G110" s="10" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="11" t="s">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A111" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B110" t="s">
-        <v>52</v>
-      </c>
-      <c r="E110" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F110" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G110" s="10" t="s">
+      <c r="B111" t="s">
+        <v>52</v>
+      </c>
+      <c r="E111" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F111" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G111" s="10" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="11" t="s">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A112" s="11" t="s">
         <v>264</v>
       </c>
-      <c r="B111" t="s">
-        <v>52</v>
-      </c>
-      <c r="E111" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F111" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G111" s="10" t="s">
+      <c r="B112" t="s">
+        <v>52</v>
+      </c>
+      <c r="E112" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F112" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G112" s="10" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="11" t="s">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A113" s="11" t="s">
         <v>266</v>
       </c>
-      <c r="B112" t="s">
-        <v>52</v>
-      </c>
-      <c r="E112" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F112" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G112" s="10" t="s">
+      <c r="B113" t="s">
+        <v>52</v>
+      </c>
+      <c r="E113" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F113" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G113" s="10" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" s="11" t="s">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A114" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="B113" t="s">
-        <v>52</v>
-      </c>
-      <c r="E113" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F113" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G113" s="10" t="s">
+      <c r="B114" t="s">
+        <v>52</v>
+      </c>
+      <c r="E114" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F114" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G114" s="10" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="11" t="s">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A115" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="B114" t="s">
-        <v>52</v>
-      </c>
-      <c r="E114" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="F114" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G114" s="10" t="s">
+      <c r="B115" t="s">
+        <v>52</v>
+      </c>
+      <c r="E115" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="F115" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G115" s="10" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
         <v>272</v>
       </c>
-      <c r="B115" t="s">
-        <v>52</v>
-      </c>
-      <c r="E115" t="s">
+      <c r="B116" t="s">
+        <v>52</v>
+      </c>
+      <c r="E116" t="s">
         <v>273</v>
       </c>
-      <c r="G115" t="s">
+      <c r="G116" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="11" t="s">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A117" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="B116" t="s">
-        <v>52</v>
-      </c>
-      <c r="E116" t="s">
-        <v>201</v>
-      </c>
-      <c r="F116" t="s">
-        <v>25</v>
-      </c>
-      <c r="G116" s="10" t="s">
+      <c r="B117" t="s">
+        <v>52</v>
+      </c>
+      <c r="E117" t="s">
+        <v>201</v>
+      </c>
+      <c r="F117" t="s">
+        <v>25</v>
+      </c>
+      <c r="G117" s="10" t="s">
         <v>276</v>
       </c>
     </row>
@@ -3420,79 +3448,79 @@
     <hyperlink ref="G14" r:id="rId2"/>
     <hyperlink ref="G13" r:id="rId3"/>
     <hyperlink ref="G12" r:id="rId4"/>
-    <hyperlink ref="G35" r:id="rId5"/>
-    <hyperlink ref="G36" r:id="rId6"/>
-    <hyperlink ref="G37" r:id="rId7"/>
-    <hyperlink ref="G38" r:id="rId8"/>
-    <hyperlink ref="G40" r:id="rId9"/>
-    <hyperlink ref="G41" r:id="rId10"/>
-    <hyperlink ref="G42" r:id="rId11"/>
-    <hyperlink ref="G46" r:id="rId12"/>
-    <hyperlink ref="G47" r:id="rId13"/>
-    <hyperlink ref="G48" r:id="rId14"/>
-    <hyperlink ref="G49" r:id="rId15"/>
-    <hyperlink ref="G50" r:id="rId16"/>
-    <hyperlink ref="G52" r:id="rId17"/>
-    <hyperlink ref="G56" r:id="rId18"/>
-    <hyperlink ref="G55" r:id="rId19"/>
-    <hyperlink ref="G57" r:id="rId20"/>
-    <hyperlink ref="G58" r:id="rId21"/>
-    <hyperlink ref="G59" r:id="rId22"/>
-    <hyperlink ref="G60" r:id="rId23"/>
-    <hyperlink ref="G61" r:id="rId24"/>
-    <hyperlink ref="G62" r:id="rId25"/>
-    <hyperlink ref="G63" r:id="rId26"/>
-    <hyperlink ref="G64" r:id="rId27"/>
-    <hyperlink ref="G65" r:id="rId28"/>
-    <hyperlink ref="G66" r:id="rId29"/>
-    <hyperlink ref="G67" r:id="rId30"/>
-    <hyperlink ref="G68" r:id="rId31"/>
-    <hyperlink ref="G69" r:id="rId32"/>
-    <hyperlink ref="G70" r:id="rId33"/>
-    <hyperlink ref="G54" r:id="rId34"/>
-    <hyperlink ref="G71" r:id="rId35"/>
-    <hyperlink ref="G72" r:id="rId36"/>
-    <hyperlink ref="G73" r:id="rId37"/>
-    <hyperlink ref="G74" r:id="rId38"/>
-    <hyperlink ref="G75" r:id="rId39"/>
-    <hyperlink ref="G76" r:id="rId40"/>
-    <hyperlink ref="G77" r:id="rId41"/>
-    <hyperlink ref="G78" r:id="rId42"/>
-    <hyperlink ref="G79" r:id="rId43"/>
-    <hyperlink ref="G80" r:id="rId44"/>
-    <hyperlink ref="G81" r:id="rId45"/>
-    <hyperlink ref="G83" r:id="rId46"/>
-    <hyperlink ref="G84" r:id="rId47"/>
-    <hyperlink ref="G85" r:id="rId48"/>
-    <hyperlink ref="G86" r:id="rId49"/>
-    <hyperlink ref="G87" r:id="rId50"/>
-    <hyperlink ref="G88" r:id="rId51"/>
-    <hyperlink ref="G89" r:id="rId52"/>
-    <hyperlink ref="G90" r:id="rId53"/>
-    <hyperlink ref="G91" r:id="rId54"/>
-    <hyperlink ref="G92" r:id="rId55"/>
-    <hyperlink ref="G93" r:id="rId56"/>
-    <hyperlink ref="G94" r:id="rId57"/>
-    <hyperlink ref="G95" r:id="rId58"/>
-    <hyperlink ref="G96" r:id="rId59"/>
-    <hyperlink ref="G97" r:id="rId60"/>
-    <hyperlink ref="G98" r:id="rId61"/>
-    <hyperlink ref="G99" r:id="rId62"/>
-    <hyperlink ref="G100" r:id="rId63"/>
-    <hyperlink ref="G101" r:id="rId64"/>
-    <hyperlink ref="G102" r:id="rId65"/>
-    <hyperlink ref="G103" r:id="rId66"/>
-    <hyperlink ref="G104" r:id="rId67"/>
-    <hyperlink ref="G105" r:id="rId68"/>
-    <hyperlink ref="G106" r:id="rId69"/>
-    <hyperlink ref="G107" r:id="rId70"/>
-    <hyperlink ref="G108" r:id="rId71"/>
-    <hyperlink ref="G109" r:id="rId72"/>
-    <hyperlink ref="G110" r:id="rId73"/>
-    <hyperlink ref="G111" r:id="rId74"/>
-    <hyperlink ref="G114" r:id="rId75"/>
-    <hyperlink ref="G112" r:id="rId76" display="AssetPageUser1@mailinator.com "/>
-    <hyperlink ref="G116" r:id="rId77"/>
+    <hyperlink ref="G36" r:id="rId5"/>
+    <hyperlink ref="G37" r:id="rId6"/>
+    <hyperlink ref="G38" r:id="rId7"/>
+    <hyperlink ref="G39" r:id="rId8"/>
+    <hyperlink ref="G41" r:id="rId9"/>
+    <hyperlink ref="G42" r:id="rId10"/>
+    <hyperlink ref="G43" r:id="rId11"/>
+    <hyperlink ref="G47" r:id="rId12"/>
+    <hyperlink ref="G48" r:id="rId13"/>
+    <hyperlink ref="G49" r:id="rId14"/>
+    <hyperlink ref="G50" r:id="rId15"/>
+    <hyperlink ref="G51" r:id="rId16"/>
+    <hyperlink ref="G53" r:id="rId17"/>
+    <hyperlink ref="G57" r:id="rId18"/>
+    <hyperlink ref="G56" r:id="rId19"/>
+    <hyperlink ref="G58" r:id="rId20"/>
+    <hyperlink ref="G59" r:id="rId21"/>
+    <hyperlink ref="G60" r:id="rId22"/>
+    <hyperlink ref="G61" r:id="rId23"/>
+    <hyperlink ref="G62" r:id="rId24"/>
+    <hyperlink ref="G63" r:id="rId25"/>
+    <hyperlink ref="G64" r:id="rId26"/>
+    <hyperlink ref="G65" r:id="rId27"/>
+    <hyperlink ref="G66" r:id="rId28"/>
+    <hyperlink ref="G67" r:id="rId29"/>
+    <hyperlink ref="G68" r:id="rId30"/>
+    <hyperlink ref="G69" r:id="rId31"/>
+    <hyperlink ref="G70" r:id="rId32"/>
+    <hyperlink ref="G71" r:id="rId33"/>
+    <hyperlink ref="G55" r:id="rId34"/>
+    <hyperlink ref="G72" r:id="rId35"/>
+    <hyperlink ref="G73" r:id="rId36"/>
+    <hyperlink ref="G74" r:id="rId37"/>
+    <hyperlink ref="G75" r:id="rId38"/>
+    <hyperlink ref="G76" r:id="rId39"/>
+    <hyperlink ref="G77" r:id="rId40"/>
+    <hyperlink ref="G78" r:id="rId41"/>
+    <hyperlink ref="G79" r:id="rId42"/>
+    <hyperlink ref="G80" r:id="rId43"/>
+    <hyperlink ref="G81" r:id="rId44"/>
+    <hyperlink ref="G82" r:id="rId45"/>
+    <hyperlink ref="G84" r:id="rId46"/>
+    <hyperlink ref="G85" r:id="rId47"/>
+    <hyperlink ref="G86" r:id="rId48"/>
+    <hyperlink ref="G87" r:id="rId49"/>
+    <hyperlink ref="G88" r:id="rId50"/>
+    <hyperlink ref="G89" r:id="rId51"/>
+    <hyperlink ref="G90" r:id="rId52"/>
+    <hyperlink ref="G91" r:id="rId53"/>
+    <hyperlink ref="G92" r:id="rId54"/>
+    <hyperlink ref="G93" r:id="rId55"/>
+    <hyperlink ref="G94" r:id="rId56"/>
+    <hyperlink ref="G95" r:id="rId57"/>
+    <hyperlink ref="G96" r:id="rId58"/>
+    <hyperlink ref="G97" r:id="rId59"/>
+    <hyperlink ref="G98" r:id="rId60"/>
+    <hyperlink ref="G99" r:id="rId61"/>
+    <hyperlink ref="G100" r:id="rId62"/>
+    <hyperlink ref="G101" r:id="rId63"/>
+    <hyperlink ref="G102" r:id="rId64"/>
+    <hyperlink ref="G103" r:id="rId65"/>
+    <hyperlink ref="G104" r:id="rId66"/>
+    <hyperlink ref="G105" r:id="rId67"/>
+    <hyperlink ref="G106" r:id="rId68"/>
+    <hyperlink ref="G107" r:id="rId69"/>
+    <hyperlink ref="G108" r:id="rId70"/>
+    <hyperlink ref="G109" r:id="rId71"/>
+    <hyperlink ref="G110" r:id="rId72"/>
+    <hyperlink ref="G111" r:id="rId73"/>
+    <hyperlink ref="G112" r:id="rId74"/>
+    <hyperlink ref="G115" r:id="rId75"/>
+    <hyperlink ref="G113" r:id="rId76" display="AssetPageUser1@mailinator.com "/>
+    <hyperlink ref="G117" r:id="rId77"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId78"/>
@@ -3507,13 +3535,13 @@
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>67</v>
       </c>
@@ -3521,7 +3549,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>203</v>
       </c>
@@ -3529,7 +3557,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>205</v>
       </c>
@@ -3548,7 +3576,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>